<commit_message>
Cambios realizador por Angel Waidelich, correcion de errores y cambios en vision y mision
</commit_message>
<xml_diff>
--- a/public/correlativas/correlativas-sistemas.xlsx
+++ b/public/correlativas/correlativas-sistemas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waide\Documents\isippweb\public\correlativas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waide\OneDrive\Documentos\isippweb\public\correlativas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B128AF-D36E-452D-9A2A-4522578D19BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7691DD-3C28-4F1E-91DA-480650C959EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2A5216C-308D-485F-86EC-E102D64CDF82}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Materia</t>
   </si>
@@ -42,107 +42,104 @@
     <t>Cuatrimestre</t>
   </si>
   <si>
-    <t>Matematicas</t>
-  </si>
-  <si>
     <t>Anual</t>
   </si>
   <si>
-    <t>Ingles</t>
-  </si>
-  <si>
-    <t>Filosofia</t>
-  </si>
-  <si>
-    <t>Diagramacion y metodo</t>
-  </si>
-  <si>
-    <t>Sistema de computacion</t>
-  </si>
-  <si>
-    <t>cuatrimestral</t>
-  </si>
-  <si>
-    <t>Sistema operativo</t>
-  </si>
-  <si>
-    <t>Analisis matematico</t>
-  </si>
-  <si>
-    <t>desarrollo de aplicaciones</t>
-  </si>
-  <si>
-    <t>Ingles,Diagramacion y metodo,Sistema operativo</t>
-  </si>
-  <si>
-    <t>lenguaje de programacion</t>
-  </si>
-  <si>
-    <t>Redes y Comunicación</t>
-  </si>
-  <si>
     <t>Organización contable</t>
   </si>
   <si>
     <t>Base de datos</t>
   </si>
   <si>
-    <t>desarrollo de aplicaciones. lenguaje de programacion, Redes y Comunicación</t>
-  </si>
-  <si>
-    <t>Desarrollo dis. Imp</t>
-  </si>
-  <si>
-    <t>desarrollo de aplicaciones. lenguaje de programacion,Redes y Comunicación</t>
-  </si>
-  <si>
-    <t>Orquestacion</t>
-  </si>
-  <si>
-    <t>Metodo Numerico</t>
-  </si>
-  <si>
-    <t>Etica y Deontologia profesional</t>
-  </si>
-  <si>
-    <t>Piscologia Organizacional</t>
-  </si>
-  <si>
-    <t>Estadisticas y probabilidad</t>
-  </si>
-  <si>
-    <t>Matematicas Financiera</t>
-  </si>
-  <si>
-    <t>Analisis de sistema</t>
-  </si>
-  <si>
-    <t>Consultoria</t>
-  </si>
-  <si>
     <t>Arquitectura de software</t>
   </si>
   <si>
-    <t>Practicas Profesionalizantes</t>
-  </si>
-  <si>
-    <t>Organización contable,Base de datos,desarrollo de aplicaciones,lenguaje de programacion</t>
-  </si>
-  <si>
-    <t>Investigacion Operativa</t>
-  </si>
-  <si>
-    <t>Metodo Numerico,Organización contable</t>
-  </si>
-  <si>
-    <t>Analisis de sistema,Matematicas Financiera,Consultoria,Arquitectura de software,Piscologia Organizacional</t>
+    <t>Sistema operativo y herramientas de productividad</t>
+  </si>
+  <si>
+    <t>Matemáticas</t>
+  </si>
+  <si>
+    <t>Inglés</t>
+  </si>
+  <si>
+    <t>Filosofía</t>
+  </si>
+  <si>
+    <t>Diagramación y método</t>
+  </si>
+  <si>
+    <t>Sistema de computación</t>
+  </si>
+  <si>
+    <t>Cuatrimestral</t>
+  </si>
+  <si>
+    <t>Análisis matemático</t>
+  </si>
+  <si>
+    <t>Desarrollo de aplicaciones</t>
+  </si>
+  <si>
+    <t>Inglés, Diagramación y método, Sistema operativo y herramientas de productividad</t>
+  </si>
+  <si>
+    <t>Lenguaje de programación</t>
+  </si>
+  <si>
+    <t>Redes y comunicación</t>
+  </si>
+  <si>
+    <t>Desarrollo de aplicaciones, Lenguaje de programación, Redes y comunicación</t>
+  </si>
+  <si>
+    <t>Desarrollo de sistemas de impresión</t>
+  </si>
+  <si>
+    <t>Orquestación</t>
+  </si>
+  <si>
+    <t>Método numérico</t>
+  </si>
+  <si>
+    <t>Ética y deontología profesional</t>
+  </si>
+  <si>
+    <t>Psicología organizacional</t>
+  </si>
+  <si>
+    <t>Estadísticas y probabilidad</t>
+  </si>
+  <si>
+    <t>Matemática financiera</t>
+  </si>
+  <si>
+    <t>Análisis de sistemas</t>
+  </si>
+  <si>
+    <t>Organización contable, Base de datos, Desarrollo de aplicaciones, Lenguaje de programación</t>
+  </si>
+  <si>
+    <t>Consultoría</t>
+  </si>
+  <si>
+    <t>Investigación operativa</t>
+  </si>
+  <si>
+    <t>Método numérico, Organización contable</t>
+  </si>
+  <si>
+    <t>Prácticas profesionalizantes</t>
+  </si>
+  <si>
+    <t>Análisis de sistemas, Matemática financiera, Consultoría, Arquitectura de software, Psicología organizacional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,14 +149,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,16 +176,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -515,13 +500,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157ABB6C-B35C-4F51-AF68-5CA2FC9FB679}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E26" sqref="A26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,206 +519,210 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2">
         <v>2</v>
       </c>
     </row>
@@ -745,12 +734,12 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
@@ -762,12 +751,12 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
         <v>2</v>
       </c>
     </row>
@@ -779,12 +768,12 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2">
         <v>1</v>
       </c>
     </row>
@@ -799,9 +788,9 @@
         <v>25</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="3">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2">
         <v>2</v>
       </c>
     </row>
@@ -813,16 +802,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -830,16 +819,16 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -847,50 +836,63 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
-        <v>33</v>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -901,25 +903,17 @@
         <v>35</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="2">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Añadicion de, institucional la seccion con mision y vision, historia re ubicada y desarrollado por, ademas de unificar contacto con ubicacion, ademas de una reinvencion del sistema de correlativas
</commit_message>
<xml_diff>
--- a/public/correlativas/correlativas-sistemas.xlsx
+++ b/public/correlativas/correlativas-sistemas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waide\OneDrive\Documentos\isippweb\public\correlativas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waide\Downloads\isippweb\public\correlativas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7691DD-3C28-4F1E-91DA-480650C959EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B823A2-CC0B-4D6C-9479-27096C840457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2A5216C-308D-485F-86EC-E102D64CDF82}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>Materia</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Año</t>
   </si>
   <si>
-    <t>Correlativas</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -45,94 +42,115 @@
     <t>Anual</t>
   </si>
   <si>
-    <t>Organización contable</t>
-  </si>
-  <si>
-    <t>Base de datos</t>
-  </si>
-  <si>
-    <t>Arquitectura de software</t>
-  </si>
-  <si>
-    <t>Sistema operativo y herramientas de productividad</t>
-  </si>
-  <si>
-    <t>Matemáticas</t>
-  </si>
-  <si>
-    <t>Inglés</t>
-  </si>
-  <si>
-    <t>Filosofía</t>
-  </si>
-  <si>
-    <t>Diagramación y método</t>
-  </si>
-  <si>
-    <t>Sistema de computación</t>
-  </si>
-  <si>
     <t>Cuatrimestral</t>
   </si>
   <si>
-    <t>Análisis matemático</t>
-  </si>
-  <si>
-    <t>Desarrollo de aplicaciones</t>
-  </si>
-  <si>
-    <t>Inglés, Diagramación y método, Sistema operativo y herramientas de productividad</t>
-  </si>
-  <si>
-    <t>Lenguaje de programación</t>
-  </si>
-  <si>
-    <t>Redes y comunicación</t>
-  </si>
-  <si>
-    <t>Desarrollo de aplicaciones, Lenguaje de programación, Redes y comunicación</t>
-  </si>
-  <si>
-    <t>Desarrollo de sistemas de impresión</t>
-  </si>
-  <si>
-    <t>Orquestación</t>
-  </si>
-  <si>
-    <t>Método numérico</t>
-  </si>
-  <si>
-    <t>Ética y deontología profesional</t>
-  </si>
-  <si>
     <t>Psicología organizacional</t>
   </si>
   <si>
-    <t>Estadísticas y probabilidad</t>
-  </si>
-  <si>
-    <t>Matemática financiera</t>
-  </si>
-  <si>
-    <t>Análisis de sistemas</t>
-  </si>
-  <si>
-    <t>Organización contable, Base de datos, Desarrollo de aplicaciones, Lenguaje de programación</t>
-  </si>
-  <si>
     <t>Consultoría</t>
   </si>
   <si>
     <t>Investigación operativa</t>
   </si>
   <si>
-    <t>Método numérico, Organización contable</t>
-  </si>
-  <si>
     <t>Prácticas profesionalizantes</t>
   </si>
   <si>
-    <t>Análisis de sistemas, Matemática financiera, Consultoría, Arquitectura de software, Psicología organizacional</t>
+    <t>Regularizado</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Matematicas</t>
+  </si>
+  <si>
+    <t>Ingles Tecnico</t>
+  </si>
+  <si>
+    <t>Diagramacion y Metodo</t>
+  </si>
+  <si>
+    <t>Sistema de Computacion</t>
+  </si>
+  <si>
+    <t>cuatrimestral</t>
+  </si>
+  <si>
+    <t>Sistema Operativos y Herramientas de Productividad</t>
+  </si>
+  <si>
+    <t>Analisis Matematico</t>
+  </si>
+  <si>
+    <t>Desarrollo de Aplicaciones</t>
+  </si>
+  <si>
+    <t>Ingles Tecnico,Diagramacion y Metodo,Sistema Operativos y Herramientas de Productividad</t>
+  </si>
+  <si>
+    <t>Lenguaje de Programacion</t>
+  </si>
+  <si>
+    <t>Redes y Comunicación</t>
+  </si>
+  <si>
+    <t>Base de Datos y Tecnicas de Programacion</t>
+  </si>
+  <si>
+    <t>Desarrollo de Aplicaciones, Lenguaje de Programacion, Redes y Comunicación</t>
+  </si>
+  <si>
+    <t>Orquestacion de Aplicaciones Informaticas</t>
+  </si>
+  <si>
+    <t>Analisis de Sistemas</t>
+  </si>
+  <si>
+    <t>Organización y Contabilidad</t>
+  </si>
+  <si>
+    <t>Metodos Numericos</t>
+  </si>
+  <si>
+    <t>Filosofia de la Ciencia y la Tecnica</t>
+  </si>
+  <si>
+    <t>Desarrollo Diseño e Implementacion de Aplicaciones Informaticas, Orquestacion de Aplicaciones Informaticas, Base de Datos y Tecnicas de Programacion, Organización y Contabilidad, Metodos Numericos</t>
+  </si>
+  <si>
+    <t>Desarrollo Diseño e Implementacion de Aplicaciones Informaticas</t>
+  </si>
+  <si>
+    <t>Organización y Contabilidad, Base de Datos y Tecnicas de Programacion, Desarrollo Diseño e Implementacion de Aplicaciones Informaticas, Orquestacion de Aplicaciones Informaticas</t>
+  </si>
+  <si>
+    <t>Organización y Contabilidad, Base de Datos y Tecnicas de Programacion, Desarrollo de Aplicaciones, Lenguaje de Programacion</t>
+  </si>
+  <si>
+    <t>Filosofia de la Ciencia y la Tecnica, Desarrollo Diseño e Implementacion de Aplicaciones Informaticas, Lenguaje de Programacion, Redes y Comunicación</t>
+  </si>
+  <si>
+    <t>Filosofia de la Ciencia y la Tecnica, Desarrollo de Aplicaciones, Lenguaje de Programacion, Redes y Comunicación</t>
+  </si>
+  <si>
+    <t>Ética y Deontologia Profesíonal</t>
+  </si>
+  <si>
+    <t>Metodos Numericos, Organización y Contabilidad</t>
+  </si>
+  <si>
+    <t>Estadísticas y Probabilidad</t>
+  </si>
+  <si>
+    <t>Analisis de Sistemas, Matemática Financiera, Consultoría, Arquitectura de Software, Psicología organizacional</t>
+  </si>
+  <si>
+    <t>Matemática Financiera</t>
+  </si>
+  <si>
+    <t>Arquitectura de Software</t>
   </si>
 </sst>
 </file>
@@ -498,15 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157ABB6C-B35C-4F51-AF68-5CA2FC9FB679}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E26" sqref="A26:E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,289 +532,315 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -805,111 +849,134 @@
         <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
         <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>

</xml_diff>